<commit_message>
add continuous frames annotation to datalist files
</commit_message>
<xml_diff>
--- a/datalists/HA_HD_list.xlsx
+++ b/datalists/HA_HD_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>/data2/shared/data/Results/recording31.4g100-350/recording31.4g_X1_skeletons.hdf5</t>
   </si>
@@ -52,18 +52,160 @@
   </si>
   <si>
     <t>*: phase frames estimated from average of other replicates with clear hand annotation</t>
+  </si>
+  <si>
+    <t>0-3500</t>
+  </si>
+  <si>
+    <t>3550-22500</t>
+  </si>
+  <si>
+    <t>22570-25230</t>
+  </si>
+  <si>
+    <t>25370-30230</t>
+  </si>
+  <si>
+    <t>30350-end</t>
+  </si>
+  <si>
+    <t>0-1250</t>
+  </si>
+  <si>
+    <t>1300-end</t>
+  </si>
+  <si>
+    <t>0-160</t>
+  </si>
+  <si>
+    <t>180-10000</t>
+  </si>
+  <si>
+    <t>10060-13000</t>
+  </si>
+  <si>
+    <t>13100-13480</t>
+  </si>
+  <si>
+    <t>13900-19410</t>
+  </si>
+  <si>
+    <t>19860-21940</t>
+  </si>
+  <si>
+    <t>22080-25270</t>
+  </si>
+  <si>
+    <t>25430-26700</t>
+  </si>
+  <si>
+    <t>27100-28990</t>
+  </si>
+  <si>
+    <t>0-1110</t>
+  </si>
+  <si>
+    <t>1140-18000</t>
+  </si>
+  <si>
+    <t>18060-23630</t>
+  </si>
+  <si>
+    <t>23900-27680</t>
+  </si>
+  <si>
+    <t>27800-end</t>
+  </si>
+  <si>
+    <t>0-1490</t>
+  </si>
+  <si>
+    <t>1530-19280</t>
+  </si>
+  <si>
+    <t>19410-22230</t>
+  </si>
+  <si>
+    <t>22350-23360</t>
+  </si>
+  <si>
+    <t>0-2220</t>
+  </si>
+  <si>
+    <t>2320-16000</t>
+  </si>
+  <si>
+    <t>16160-20600</t>
+  </si>
+  <si>
+    <t>20680-28420</t>
+  </si>
+  <si>
+    <t>28550-end</t>
+  </si>
+  <si>
+    <t>1540-12720</t>
+  </si>
+  <si>
+    <t>12810-18670</t>
+  </si>
+  <si>
+    <t>18830-21960</t>
+  </si>
+  <si>
+    <t>22420-end</t>
+  </si>
+  <si>
+    <t>0-690</t>
+  </si>
+  <si>
+    <t>740-13500</t>
+  </si>
+  <si>
+    <t>13620-16560</t>
+  </si>
+  <si>
+    <t>16670-19050</t>
+  </si>
+  <si>
+    <t>19230-20920</t>
+  </si>
+  <si>
+    <t>21030-22040</t>
+  </si>
+  <si>
+    <t>22200-23870</t>
+  </si>
+  <si>
+    <t>24000-25160</t>
+  </si>
+  <si>
+    <t>25380-26490</t>
+  </si>
+  <si>
+    <t>26600-end</t>
+  </si>
+  <si>
+    <t>0-17250</t>
+  </si>
+  <si>
+    <t>17400-21300</t>
+  </si>
+  <si>
+    <t>21370-21570</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -89,6 +231,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -112,9 +259,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -448,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -459,7 +607,7 @@
     <col min="1" max="1" width="73.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,8 +623,28 @@
       <c r="E1">
         <v>32400</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -492,8 +660,22 @@
       <c r="E2">
         <v>32400</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -509,8 +691,36 @@
       <c r="E3">
         <v>29211</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -529,8 +739,28 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -546,8 +776,26 @@
       <c r="E5">
         <v>24303</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -566,8 +814,28 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -583,8 +851,28 @@
       <c r="E7">
         <v>24058</v>
       </c>
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -603,8 +891,38 @@
       <c r="F8" t="s">
         <v>9</v>
       </c>
+      <c r="G8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -623,6 +941,22 @@
       <c r="F9" t="s">
         <v>9</v>
       </c>
+      <c r="G9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
     </row>
     <row r="17" spans="6:6">
       <c r="F17" s="1" t="s">

</xml_diff>